<commit_message>
master_code....py: fixing some bugs, README + participants list: some minor changes
</commit_message>
<xml_diff>
--- a/participants list.xlsx
+++ b/participants list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u213619\Documents\Pep\06 World Cup 2022\WTP\Game 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u213619\Documents\Pep\06 World Cup 2022\WTP\FIFA World Cup 2022 Game - Play with your friends\FIFA-World-Cup-2022-Random-Team-Picker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AA94D3-EBD7-4BF8-916D-EF9C00F51EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3295CDE5-2D41-455F-A67C-AEB703F341C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Nombre</t>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A23:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,71 +466,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>